<commit_message>
update: integrate computer vision and data mining system into dashboard
</commit_message>
<xml_diff>
--- a/static/metadata.xlsx
+++ b/static/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alif\Music\lomba\AgriSim\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFD8A4E-993D-4696-9951-61ADCAEBD9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B61BB2-AB70-44F2-B410-64A3ED10C099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="3472" windowWidth="16200" windowHeight="9308" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="informasi umum" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Filename</t>
   </si>
@@ -46,35 +46,68 @@
     <t>komoditas tanaman</t>
   </si>
   <si>
-    <t>tanaman</t>
-  </si>
-  <si>
-    <t>harga bibit</t>
-  </si>
-  <si>
-    <t>masa panen</t>
-  </si>
-  <si>
-    <t>harga jual (kg)</t>
-  </si>
-  <si>
     <t>karawang.png</t>
   </si>
   <si>
-    <t>padi, jagung, kedelai, kacang tanah, ubi kayu, ubi jalar</t>
+    <t>padi, jagung, kacang tanah, ubi kayu, ubi jalar</t>
+  </si>
+  <si>
+    <t>Tanaman</t>
+  </si>
+  <si>
+    <t>Harga Bibit (Rp/m2)</t>
+  </si>
+  <si>
+    <t>Masa Panen (hari)</t>
+  </si>
+  <si>
+    <t>Hasil Panen (kg/m2)</t>
+  </si>
+  <si>
+    <t>Harga Jual (Rp/kg)</t>
+  </si>
+  <si>
+    <t>Padi</t>
+  </si>
+  <si>
+    <t>Jagung</t>
+  </si>
+  <si>
+    <t>Biaya Total (Rp)</t>
+  </si>
+  <si>
+    <t>Hasil Panen (Rp)</t>
+  </si>
+  <si>
+    <t>Keuntungan (Rp)</t>
+  </si>
+  <si>
+    <t>Kacang Tanah</t>
+  </si>
+  <si>
+    <t>Ubi Kayu</t>
+  </si>
+  <si>
+    <t>Ubi Jalar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,8 +130,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -409,7 +448,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>-6.3253499</v>
@@ -421,7 +460,7 @@
         <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -431,32 +470,178 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DE5D61-E4BE-4CE9-92EC-1E3FC90CF62D}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="11.53125" customWidth="1"/>
-    <col min="3" max="3" width="14.1328125" customWidth="1"/>
-    <col min="4" max="4" width="19.1328125" customWidth="1"/>
-    <col min="5" max="5" width="9.06640625" customWidth="1"/>
+    <col min="1" max="1" width="14.73046875" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
+    <col min="3" max="3" width="15.9296875" customWidth="1"/>
+    <col min="4" max="4" width="18.3984375" customWidth="1"/>
+    <col min="5" max="5" width="15.9296875" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="7" max="7" width="14.9296875" customWidth="1"/>
+    <col min="8" max="8" width="16.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2">
+        <v>120</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2">
+        <v>600</v>
+      </c>
+      <c r="G2" s="2">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
+        <v>300</v>
+      </c>
+      <c r="G3" s="2">
+        <v>60</v>
+      </c>
+      <c r="H3" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2">
+        <v>120</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2">
+        <v>375</v>
+      </c>
+      <c r="G4" s="2">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>120</v>
+      </c>
+      <c r="D5" s="2">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>50</v>
+      </c>
+      <c r="H5" s="2">
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>100</v>
+      </c>
+      <c r="D6" s="2">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>150</v>
+      </c>
+      <c r="H6" s="2">
+        <v>138.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>